<commit_message>
updated with threadlocal for execution performance along with parallel execution
</commit_message>
<xml_diff>
--- a/src/main/resources/excels/testdata.xlsx
+++ b/src/main/resources/excels/testdata.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Selenium_Class\diathrive\src\main\resources\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\diathrive_framework\diathrive\diathrive\src\main\resources\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB9A5A2-A445-42FC-B867-F5B5AC62C75C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>firstname</t>
   </si>
@@ -108,17 +107,17 @@
     <t>password</t>
   </si>
   <si>
-    <t>khaleelshaik2711@gmail.com</t>
-  </si>
-  <si>
-    <t>Abcd#123E</t>
+    <t>ravinskanni@gmail.com</t>
+  </si>
+  <si>
+    <t>abcd@123E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +130,14 @@
       <color rgb="FF2A00FF"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -150,16 +157,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -437,7 +449,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -487,7 +499,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -587,7 +599,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -621,11 +633,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE45DF17-CDA5-4497-86AC-8CEF02C4087B}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,15 +655,27 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>